<commit_message>
Agregado modulo de inventario aun me falta darle formato para que guarde los item Tambien los ejs
</commit_message>
<xml_diff>
--- a/archivos/CAR01 PS001.xlsx
+++ b/archivos/CAR01 PS001.xlsx
@@ -5,16 +5,16 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PARKING SOLUTIONS\MATTO PERS\PLAN DE MANTENIMIENTO\PLAN ANUAL EXCEL 2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\APP\ordenes\archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="24585" windowHeight="14460" tabRatio="801" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="24585" windowHeight="14460" tabRatio="801"/>
   </bookViews>
   <sheets>
-    <sheet name="COSTOS" sheetId="19" state="hidden" r:id="rId1"/>
-    <sheet name="TIEMPOS" sheetId="20" state="hidden" r:id="rId2"/>
-    <sheet name="HORAS HOMBRE" sheetId="28" state="hidden" r:id="rId3"/>
+    <sheet name="COSTOS" sheetId="19" r:id="rId1"/>
+    <sheet name="TIEMPOS" sheetId="20" r:id="rId2"/>
+    <sheet name="HORAS HOMBRE" sheetId="28" r:id="rId3"/>
     <sheet name="PREVENTIVO" sheetId="33" r:id="rId4"/>
     <sheet name="AÑO 7" sheetId="30" r:id="rId5"/>
   </sheets>
@@ -28,7 +28,7 @@
     <definedName name="RepuestosGarantiaAño7">'AÑO 7'!$C$33:$G$52</definedName>
     <definedName name="TiempoRepuesto">Tbl_TiempoRespuestos[[CAMBIO DE REPUESTOS ]]</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -706,16 +706,16 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="8">
-    <numFmt numFmtId="44" formatCode="_-&quot;S/&quot;* #,##0.00_-;\-&quot;S/&quot;* #,##0.00_-;_-&quot;S/&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_ &quot;S/&quot;\ * #,##0.00_ ;_ &quot;S/&quot;\ * \-#,##0.00_ ;_ &quot;S/&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="165" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="166" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="167" formatCode="_ &quot;S/.&quot;\ * #,##0.00_ ;_ &quot;S/.&quot;\ * \-#,##0.00_ ;_ &quot;S/.&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="168" formatCode="_-[$$-540A]* #,##0.00_ ;_-[$$-540A]* \-#,##0.00\ ;_-[$$-540A]* &quot;-&quot;??_ ;_-@_ "/>
-    <numFmt numFmtId="169" formatCode="[$$-409]#,##0.00"/>
-    <numFmt numFmtId="170" formatCode="[h]:mm"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;S/&quot;* #,##0.00_-;\-&quot;S/&quot;* #,##0.00_-;_-&quot;S/&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_ &quot;S/&quot;\ * #,##0.00_ ;_ &quot;S/&quot;\ * \-#,##0.00_ ;_ &quot;S/&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="166" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="167" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="168" formatCode="_ &quot;S/.&quot;\ * #,##0.00_ ;_ &quot;S/.&quot;\ * \-#,##0.00_ ;_ &quot;S/.&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="169" formatCode="_-[$$-540A]* #,##0.00_ ;_-[$$-540A]* \-#,##0.00\ ;_-[$$-540A]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="170" formatCode="[$$-409]#,##0.00"/>
+    <numFmt numFmtId="171" formatCode="[h]:mm"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -1249,12 +1249,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="173">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1274,7 +1274,7 @@
     <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="112" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="112" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="112" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1290,18 +1290,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1310,48 +1310,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="113" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="170" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="10" borderId="0" xfId="113" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="113" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="10" borderId="0" xfId="113" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="20" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1391,9 +1391,9 @@
     <xf numFmtId="2" fontId="11" fillId="2" borderId="1" xfId="112" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
@@ -1426,7 +1426,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1462,28 +1462,28 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="170" fontId="7" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="7" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1531,7 +1531,7 @@
     <xf numFmtId="0" fontId="12" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="12" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="12" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1551,7 +1551,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="8" fillId="5" borderId="1" xfId="112" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="8" fillId="5" borderId="1" xfId="112" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1560,7 +1560,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="5" borderId="10" xfId="112" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="8" fillId="5" borderId="10" xfId="112" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1570,119 +1570,119 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="114">
@@ -1823,37 +1823,37 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_ &quot;S/&quot;\ * #,##0.00_ ;_ &quot;S/&quot;\ * \-#,##0.00_ ;_ &quot;S/&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+      <numFmt numFmtId="165" formatCode="_ &quot;S/&quot;\ * #,##0.00_ ;_ &quot;S/&quot;\ * \-#,##0.00_ ;_ &quot;S/&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_ &quot;S/&quot;\ * #,##0.00_ ;_ &quot;S/&quot;\ * \-#,##0.00_ ;_ &quot;S/&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+      <numFmt numFmtId="165" formatCode="_ &quot;S/&quot;\ * #,##0.00_ ;_ &quot;S/&quot;\ * \-#,##0.00_ ;_ &quot;S/&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_ &quot;S/&quot;\ * #,##0.00_ ;_ &quot;S/&quot;\ * \-#,##0.00_ ;_ &quot;S/&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+      <numFmt numFmtId="165" formatCode="_ &quot;S/&quot;\ * #,##0.00_ ;_ &quot;S/&quot;\ * \-#,##0.00_ ;_ &quot;S/&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_ &quot;S/&quot;\ * #,##0.00_ ;_ &quot;S/&quot;\ * \-#,##0.00_ ;_ &quot;S/&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+      <numFmt numFmtId="165" formatCode="_ &quot;S/&quot;\ * #,##0.00_ ;_ &quot;S/&quot;\ * \-#,##0.00_ ;_ &quot;S/&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_ &quot;S/&quot;\ * #,##0.00_ ;_ &quot;S/&quot;\ * \-#,##0.00_ ;_ &quot;S/&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+      <numFmt numFmtId="165" formatCode="_ &quot;S/&quot;\ * #,##0.00_ ;_ &quot;S/&quot;\ * \-#,##0.00_ ;_ &quot;S/&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_ &quot;S/&quot;\ * #,##0.00_ ;_ &quot;S/&quot;\ * \-#,##0.00_ ;_ &quot;S/&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+      <numFmt numFmtId="165" formatCode="_ &quot;S/&quot;\ * #,##0.00_ ;_ &quot;S/&quot;\ * \-#,##0.00_ ;_ &quot;S/&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_ &quot;S/&quot;\ * #,##0.00_ ;_ &quot;S/&quot;\ * \-#,##0.00_ ;_ &quot;S/&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+      <numFmt numFmtId="165" formatCode="_ &quot;S/&quot;\ * #,##0.00_ ;_ &quot;S/&quot;\ * \-#,##0.00_ ;_ &quot;S/&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_ &quot;S/&quot;\ * #,##0.00_ ;_ &quot;S/&quot;\ * \-#,##0.00_ ;_ &quot;S/&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+      <numFmt numFmtId="165" formatCode="_ &quot;S/&quot;\ * #,##0.00_ ;_ &quot;S/&quot;\ * \-#,##0.00_ ;_ &quot;S/&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_ &quot;S/&quot;\ * #,##0.00_ ;_ &quot;S/&quot;\ * \-#,##0.00_ ;_ &quot;S/&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+      <numFmt numFmtId="165" formatCode="_ &quot;S/&quot;\ * #,##0.00_ ;_ &quot;S/&quot;\ * \-#,##0.00_ ;_ &quot;S/&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_ &quot;S/&quot;\ * #,##0.00_ ;_ &quot;S/&quot;\ * \-#,##0.00_ ;_ &quot;S/&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+      <numFmt numFmtId="165" formatCode="_ &quot;S/&quot;\ * #,##0.00_ ;_ &quot;S/&quot;\ * \-#,##0.00_ ;_ &quot;S/&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="_-[$$-540A]* #,##0.00_ ;_-[$$-540A]* \-#,##0.00\ ;_-[$$-540A]* &quot;-&quot;??_ ;_-@_ "/>
+      <numFmt numFmtId="169" formatCode="_-[$$-540A]* #,##0.00_ ;_-[$$-540A]* \-#,##0.00\ ;_-[$$-540A]* &quot;-&quot;??_ ;_-@_ "/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1955,7 +1955,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="_-[$$-540A]* #,##0.00_ ;_-[$$-540A]* \-#,##0.00\ ;_-[$$-540A]* &quot;-&quot;??_ ;_-@_ "/>
+      <numFmt numFmtId="169" formatCode="_-[$$-540A]* #,##0.00_ ;_-[$$-540A]* \-#,##0.00\ ;_-[$$-540A]* &quot;-&quot;??_ ;_-@_ "/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -2042,7 +2042,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
+      <numFmt numFmtId="172" formatCode="hh:mm"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
@@ -2127,7 +2127,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;S/&quot;* #,##0.00_-;\-&quot;S/&quot;* #,##0.00_-;_-&quot;S/&quot;* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-&quot;S/&quot;* #,##0.00_-;\-&quot;S/&quot;* #,##0.00_-;_-&quot;S/&quot;* &quot;-&quot;??_-;_-@_-"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -2212,7 +2212,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;S/&quot;* #,##0.00_-;\-&quot;S/&quot;* #,##0.00_-;_-&quot;S/&quot;* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-&quot;S/&quot;* #,##0.00_-;\-&quot;S/&quot;* #,##0.00_-;_-&quot;S/&quot;* &quot;-&quot;??_-;_-@_-"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -2227,7 +2227,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="_-[$$-540A]* #,##0.00_ ;_-[$$-540A]* \-#,##0.00\ ;_-[$$-540A]* &quot;-&quot;??_ ;_-@_ "/>
+      <numFmt numFmtId="169" formatCode="_-[$$-540A]* #,##0.00_ ;_-[$$-540A]* \-#,##0.00\ ;_-[$$-540A]* &quot;-&quot;??_ ;_-@_ "/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -2242,7 +2242,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="_-[$$-540A]* #,##0.00_ ;_-[$$-540A]* \-#,##0.00\ ;_-[$$-540A]* &quot;-&quot;??_ ;_-@_ "/>
+      <numFmt numFmtId="169" formatCode="_-[$$-540A]* #,##0.00_ ;_-[$$-540A]* \-#,##0.00\ ;_-[$$-540A]* &quot;-&quot;??_ ;_-@_ "/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -2329,7 +2329,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;S/&quot;* #,##0.00_-;\-&quot;S/&quot;* #,##0.00_-;_-&quot;S/&quot;* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-&quot;S/&quot;* #,##0.00_-;\-&quot;S/&quot;* #,##0.00_-;_-&quot;S/&quot;* &quot;-&quot;??_-;_-@_-"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -2900,8 +2900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M41"/>
   <sheetViews>
-    <sheetView topLeftCell="D16" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3834,7 +3834,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J40"/>
   <sheetViews>
-    <sheetView topLeftCell="C4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
@@ -4448,7 +4448,7 @@
   <dimension ref="A2:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4737,7 +4737,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J52"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
@@ -4782,16 +4782,16 @@
       <c r="C5" s="104"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="135" t="s">
+      <c r="B6" s="136" t="s">
         <v>162</v>
       </c>
-      <c r="C6" s="135"/>
-      <c r="D6" s="135"/>
-      <c r="E6" s="135"/>
-      <c r="F6" s="135"/>
-      <c r="G6" s="135"/>
-      <c r="H6" s="135"/>
-      <c r="I6" s="135"/>
+      <c r="C6" s="136"/>
+      <c r="D6" s="136"/>
+      <c r="E6" s="136"/>
+      <c r="F6" s="136"/>
+      <c r="G6" s="136"/>
+      <c r="H6" s="136"/>
+      <c r="I6" s="136"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="105" t="s">
@@ -5415,8 +5415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P133"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5440,20 +5440,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="166" t="s">
+      <c r="B2" s="158" t="s">
         <v>183</v>
       </c>
-      <c r="C2" s="166"/>
+      <c r="C2" s="158"/>
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B3" s="167" t="s">
+      <c r="B3" s="159" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="167"/>
+      <c r="C3" s="159"/>
       <c r="D3" s="128" t="s">
         <v>184</v>
       </c>
@@ -5462,10 +5462,10 @@
       <c r="G3" s="5"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="167" t="s">
+      <c r="B4" s="159" t="s">
         <v>121</v>
       </c>
-      <c r="C4" s="167"/>
+      <c r="C4" s="159"/>
       <c r="D4" s="131" t="s">
         <v>185</v>
       </c>
@@ -5474,10 +5474,10 @@
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="168" t="s">
+      <c r="B5" s="160" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="168"/>
+      <c r="C5" s="160"/>
       <c r="D5" s="71">
         <v>12</v>
       </c>
@@ -5493,14 +5493,14 @@
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="161" t="s">
+      <c r="B7" s="155" t="s">
         <v>186</v>
       </c>
-      <c r="C7" s="161"/>
-      <c r="D7" s="161"/>
-      <c r="E7" s="161"/>
-      <c r="F7" s="161"/>
-      <c r="G7" s="161"/>
+      <c r="C7" s="155"/>
+      <c r="D7" s="155"/>
+      <c r="E7" s="155"/>
+      <c r="F7" s="155"/>
+      <c r="G7" s="155"/>
       <c r="I7" s="68" t="s">
         <v>9</v>
       </c>
@@ -5511,12 +5511,12 @@
       <c r="E8" s="9"/>
       <c r="F8" s="5"/>
       <c r="G8" s="10"/>
-      <c r="I8" s="169" t="s">
+      <c r="I8" s="154" t="s">
         <v>142</v>
       </c>
-      <c r="J8" s="169"/>
-      <c r="K8" s="169"/>
-      <c r="L8" s="169"/>
+      <c r="J8" s="154"/>
+      <c r="K8" s="154"/>
+      <c r="L8" s="154"/>
       <c r="M8" s="69" t="s">
         <v>10</v>
       </c>
@@ -5531,10 +5531,10 @@
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="162" t="s">
+      <c r="B9" s="156" t="s">
         <v>122</v>
       </c>
-      <c r="C9" s="163"/>
+      <c r="C9" s="157"/>
       <c r="D9" s="83"/>
       <c r="E9" s="83"/>
       <c r="F9" s="83"/>
@@ -5579,12 +5579,12 @@
       <c r="G10" s="76">
         <v>2</v>
       </c>
-      <c r="I10" s="142" t="s">
+      <c r="I10" s="141" t="s">
         <v>17</v>
       </c>
-      <c r="J10" s="142"/>
-      <c r="K10" s="142"/>
-      <c r="L10" s="142"/>
+      <c r="J10" s="141"/>
+      <c r="K10" s="141"/>
+      <c r="L10" s="141"/>
       <c r="M10" s="139"/>
       <c r="N10" s="140"/>
       <c r="O10" s="140"/>
@@ -5646,12 +5646,12 @@
         <f>G11*G9</f>
         <v>1.5749999999999997</v>
       </c>
-      <c r="I12" s="142" t="s">
+      <c r="I12" s="141" t="s">
         <v>18</v>
       </c>
-      <c r="J12" s="142"/>
-      <c r="K12" s="142"/>
-      <c r="L12" s="142"/>
+      <c r="J12" s="141"/>
+      <c r="K12" s="141"/>
+      <c r="L12" s="141"/>
       <c r="M12" s="139"/>
       <c r="N12" s="140"/>
       <c r="O12" s="140"/>
@@ -5712,22 +5712,22 @@
         <f>SUM(F26:F29)</f>
         <v>0.92500000000000004</v>
       </c>
-      <c r="I14" s="142" t="s">
+      <c r="I14" s="141" t="s">
         <v>85</v>
       </c>
-      <c r="J14" s="142"/>
-      <c r="K14" s="142"/>
-      <c r="L14" s="142"/>
+      <c r="J14" s="141"/>
+      <c r="K14" s="141"/>
+      <c r="L14" s="141"/>
       <c r="M14" s="140"/>
       <c r="N14" s="140"/>
       <c r="O14" s="140"/>
       <c r="P14" s="140"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="162" t="s">
+      <c r="B15" s="156" t="s">
         <v>136</v>
       </c>
-      <c r="C15" s="163"/>
+      <c r="C15" s="157"/>
       <c r="D15" s="83"/>
       <c r="E15" s="83"/>
       <c r="F15" s="83"/>
@@ -5772,12 +5772,12 @@
         <f>TIEMPOS!J8*G15</f>
         <v>0.375</v>
       </c>
-      <c r="I16" s="142" t="s">
+      <c r="I16" s="141" t="s">
         <v>3</v>
       </c>
-      <c r="J16" s="142"/>
-      <c r="K16" s="142"/>
-      <c r="L16" s="142"/>
+      <c r="J16" s="141"/>
+      <c r="K16" s="141"/>
+      <c r="L16" s="141"/>
       <c r="M16" s="140"/>
       <c r="N16" s="140"/>
       <c r="O16" s="140"/>
@@ -5813,31 +5813,31 @@
         <f>E18*G15</f>
         <v>0.53125</v>
       </c>
-      <c r="I18" s="143" t="s">
+      <c r="I18" s="144" t="s">
         <v>68</v>
       </c>
-      <c r="J18" s="144"/>
-      <c r="K18" s="144"/>
-      <c r="L18" s="145"/>
+      <c r="J18" s="145"/>
+      <c r="K18" s="145"/>
+      <c r="L18" s="146"/>
       <c r="M18" s="42">
         <f>SUM(M9:M16)</f>
         <v>2227.6394357638883</v>
       </c>
-      <c r="N18" s="146">
+      <c r="N18" s="147">
         <f>+SUM(N9:O16)</f>
         <v>1113.8197178819441</v>
       </c>
-      <c r="O18" s="146"/>
+      <c r="O18" s="147"/>
       <c r="P18" s="29">
         <f>SUM(P9:P16)</f>
         <v>3341.4591536458329</v>
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="162" t="s">
+      <c r="B19" s="156" t="s">
         <v>141</v>
       </c>
-      <c r="C19" s="163"/>
+      <c r="C19" s="157"/>
       <c r="D19" s="83"/>
       <c r="E19" s="84"/>
       <c r="F19" s="85"/>
@@ -5847,10 +5847,10 @@
       </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B20" s="164" t="s">
+      <c r="B20" s="151" t="s">
         <v>87</v>
       </c>
-      <c r="C20" s="165"/>
+      <c r="C20" s="152"/>
       <c r="D20" s="72"/>
       <c r="E20" s="72"/>
       <c r="F20" s="72"/>
@@ -5862,22 +5862,22 @@
       </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B21" s="164" t="s">
+      <c r="B21" s="151" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="165"/>
+      <c r="C21" s="152"/>
       <c r="D21" s="72"/>
       <c r="E21" s="72"/>
       <c r="F21" s="72"/>
       <c r="G21" s="76">
         <v>1</v>
       </c>
-      <c r="I21" s="153" t="s">
+      <c r="I21" s="150" t="s">
         <v>142</v>
       </c>
-      <c r="J21" s="153"/>
-      <c r="K21" s="153"/>
-      <c r="L21" s="153"/>
+      <c r="J21" s="150"/>
+      <c r="K21" s="150"/>
+      <c r="L21" s="150"/>
       <c r="M21" s="86" t="s">
         <v>10</v>
       </c>
@@ -5892,10 +5892,10 @@
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B22" s="164" t="s">
+      <c r="B22" s="151" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="165"/>
+      <c r="C22" s="152"/>
       <c r="D22" s="72"/>
       <c r="E22" s="72"/>
       <c r="F22" s="72"/>
@@ -5933,26 +5933,26 @@
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
       <c r="G23" s="13"/>
-      <c r="I23" s="172" t="str">
+      <c r="I23" s="149" t="str">
         <f>C26</f>
         <v>Solenoide de traba</v>
       </c>
-      <c r="J23" s="172"/>
-      <c r="K23" s="172"/>
-      <c r="L23" s="172"/>
+      <c r="J23" s="149"/>
+      <c r="K23" s="149"/>
+      <c r="L23" s="149"/>
       <c r="M23" s="139"/>
       <c r="N23" s="140"/>
       <c r="O23" s="140"/>
       <c r="P23" s="140"/>
     </row>
     <row r="24" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C24" s="136" t="s">
+      <c r="C24" s="153" t="s">
         <v>187</v>
       </c>
-      <c r="D24" s="136"/>
-      <c r="E24" s="136"/>
-      <c r="F24" s="136"/>
-      <c r="G24" s="136"/>
+      <c r="D24" s="153"/>
+      <c r="E24" s="153"/>
+      <c r="F24" s="153"/>
+      <c r="G24" s="153"/>
       <c r="I24" s="89" t="s">
         <v>69</v>
       </c>
@@ -5994,20 +5994,20 @@
       <c r="G25" s="56" t="s">
         <v>87</v>
       </c>
-      <c r="I25" s="172" t="str">
+      <c r="I25" s="149" t="str">
         <f>C27</f>
         <v>Cable Flat</v>
       </c>
-      <c r="J25" s="172"/>
-      <c r="K25" s="172"/>
-      <c r="L25" s="172"/>
+      <c r="J25" s="149"/>
+      <c r="K25" s="149"/>
+      <c r="L25" s="149"/>
       <c r="M25" s="139"/>
       <c r="N25" s="140"/>
       <c r="O25" s="140"/>
       <c r="P25" s="140"/>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C26" s="171" t="s">
+      <c r="C26" s="135" t="s">
         <v>4</v>
       </c>
       <c r="D26" s="51">
@@ -6052,7 +6052,7 @@
       </c>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C27" s="171" t="s">
+      <c r="C27" s="135" t="s">
         <v>202</v>
       </c>
       <c r="D27" s="51">
@@ -6071,20 +6071,20 @@
         <f>VLOOKUP(C27,Tbl_TiempoRespuestos[],3,0)</f>
         <v>1</v>
       </c>
-      <c r="I27" s="172" t="str">
+      <c r="I27" s="149" t="str">
         <f>C28</f>
         <v>Protector de puerta (microporoso)</v>
       </c>
-      <c r="J27" s="172"/>
-      <c r="K27" s="172"/>
-      <c r="L27" s="172"/>
+      <c r="J27" s="149"/>
+      <c r="K27" s="149"/>
+      <c r="L27" s="149"/>
       <c r="M27" s="139"/>
       <c r="N27" s="140"/>
       <c r="O27" s="140"/>
       <c r="P27" s="140"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C28" s="171" t="s">
+      <c r="C28" s="135" t="s">
         <v>201</v>
       </c>
       <c r="D28" s="51">
@@ -6148,13 +6148,13 @@
         <f>VLOOKUP(C29,Tbl_TiempoRespuestos[],3,0)</f>
         <v>0</v>
       </c>
-      <c r="I29" s="170" t="str">
+      <c r="I29" s="148" t="str">
         <f>C29</f>
         <v>Seleccionar repuesto…</v>
       </c>
-      <c r="J29" s="170"/>
-      <c r="K29" s="170"/>
-      <c r="L29" s="170"/>
+      <c r="J29" s="148"/>
+      <c r="K29" s="148"/>
+      <c r="L29" s="148"/>
       <c r="M29" s="139"/>
       <c r="N29" s="140"/>
       <c r="O29" s="140"/>
@@ -6168,28 +6168,28 @@
       <c r="G30" s="59"/>
     </row>
     <row r="31" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C31" s="136" t="s">
+      <c r="C31" s="153" t="s">
         <v>138</v>
       </c>
-      <c r="D31" s="136"/>
-      <c r="E31" s="136"/>
-      <c r="F31" s="136"/>
-      <c r="G31" s="136"/>
-      <c r="I31" s="143" t="s">
+      <c r="D31" s="153"/>
+      <c r="E31" s="153"/>
+      <c r="F31" s="153"/>
+      <c r="G31" s="153"/>
+      <c r="I31" s="144" t="s">
         <v>189</v>
       </c>
-      <c r="J31" s="144"/>
-      <c r="K31" s="144"/>
-      <c r="L31" s="145"/>
+      <c r="J31" s="145"/>
+      <c r="K31" s="145"/>
+      <c r="L31" s="146"/>
       <c r="M31" s="42">
         <f>SUM(M22:M29)</f>
         <v>3444</v>
       </c>
-      <c r="N31" s="146">
+      <c r="N31" s="147">
         <f>+SUM(N22:O29)</f>
         <v>1033.1999999999998</v>
       </c>
-      <c r="O31" s="146"/>
+      <c r="O31" s="147"/>
       <c r="P31" s="29">
         <f>SUM(P22:P29)</f>
         <v>4477.2</v>
@@ -6234,12 +6234,12 @@
         <f>VLOOKUP(C33,Tbl_TiempoRespuestos[],3,0)</f>
         <v>2</v>
       </c>
-      <c r="I33" s="151" t="s">
+      <c r="I33" s="142" t="s">
         <v>150</v>
       </c>
-      <c r="J33" s="152"/>
-      <c r="K33" s="152"/>
-      <c r="L33" s="152"/>
+      <c r="J33" s="143"/>
+      <c r="K33" s="143"/>
+      <c r="L33" s="143"/>
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B34" s="118">
@@ -6263,12 +6263,12 @@
         <f>VLOOKUP(C34,Tbl_TiempoRespuestos[],3,0)</f>
         <v>2</v>
       </c>
-      <c r="I34" s="153" t="s">
+      <c r="I34" s="150" t="s">
         <v>142</v>
       </c>
-      <c r="J34" s="153"/>
-      <c r="K34" s="153"/>
-      <c r="L34" s="153"/>
+      <c r="J34" s="150"/>
+      <c r="K34" s="150"/>
+      <c r="L34" s="150"/>
       <c r="M34" s="86" t="s">
         <v>10</v>
       </c>
@@ -6351,13 +6351,13 @@
         <f>VLOOKUP(C36,Tbl_TiempoRespuestos[],3,0)</f>
         <v>1</v>
       </c>
-      <c r="I36" s="142" t="str">
+      <c r="I36" s="141" t="str">
         <f>C33</f>
         <v xml:space="preserve">Bomba hidráulica </v>
       </c>
-      <c r="J36" s="142"/>
-      <c r="K36" s="142"/>
-      <c r="L36" s="142"/>
+      <c r="J36" s="141"/>
+      <c r="K36" s="141"/>
+      <c r="L36" s="141"/>
       <c r="M36" s="139"/>
       <c r="N36" s="140"/>
       <c r="O36" s="140"/>
@@ -6432,13 +6432,13 @@
         <f>VLOOKUP(C38,Tbl_TiempoRespuestos[],3,0)</f>
         <v>1</v>
       </c>
-      <c r="I38" s="142" t="str">
+      <c r="I38" s="141" t="str">
         <f>C34</f>
         <v>Cilindro hidráulico (kit de reten y oring)</v>
       </c>
-      <c r="J38" s="142"/>
-      <c r="K38" s="142"/>
-      <c r="L38" s="142"/>
+      <c r="J38" s="141"/>
+      <c r="K38" s="141"/>
+      <c r="L38" s="141"/>
       <c r="M38" s="139"/>
       <c r="N38" s="140"/>
       <c r="O38" s="140"/>
@@ -6513,13 +6513,13 @@
         <f>VLOOKUP(C40,Tbl_TiempoRespuestos[],3,0)</f>
         <v>1</v>
       </c>
-      <c r="I40" s="142" t="str">
+      <c r="I40" s="141" t="str">
         <f>C35</f>
         <v xml:space="preserve">Contactor </v>
       </c>
-      <c r="J40" s="142"/>
-      <c r="K40" s="142"/>
-      <c r="L40" s="142"/>
+      <c r="J40" s="141"/>
+      <c r="K40" s="141"/>
+      <c r="L40" s="141"/>
       <c r="M40" s="139"/>
       <c r="N40" s="140"/>
       <c r="O40" s="140"/>
@@ -6594,13 +6594,13 @@
         <f>VLOOKUP(C42,Tbl_TiempoRespuestos[],3,0)</f>
         <v>1</v>
       </c>
-      <c r="I42" s="142" t="str">
+      <c r="I42" s="141" t="str">
         <f>C36</f>
         <v>Condensador de trabajo</v>
       </c>
-      <c r="J42" s="142"/>
-      <c r="K42" s="142"/>
-      <c r="L42" s="142"/>
+      <c r="J42" s="141"/>
+      <c r="K42" s="141"/>
+      <c r="L42" s="141"/>
       <c r="M42" s="139"/>
       <c r="N42" s="140"/>
       <c r="O42" s="140"/>
@@ -6675,13 +6675,13 @@
         <f>VLOOKUP(C44,Tbl_TiempoRespuestos[],3,0)</f>
         <v>1</v>
       </c>
-      <c r="I44" s="142" t="str">
+      <c r="I44" s="141" t="str">
         <f>C37</f>
         <v>Electrovalvula</v>
       </c>
-      <c r="J44" s="142"/>
-      <c r="K44" s="142"/>
-      <c r="L44" s="142"/>
+      <c r="J44" s="141"/>
+      <c r="K44" s="141"/>
+      <c r="L44" s="141"/>
       <c r="M44" s="139"/>
       <c r="N44" s="140"/>
       <c r="O44" s="140"/>
@@ -6756,13 +6756,13 @@
         <f>VLOOKUP(C46,Tbl_TiempoRespuestos[],3,0)</f>
         <v>1</v>
       </c>
-      <c r="I46" s="142" t="str">
+      <c r="I46" s="141" t="str">
         <f>C38</f>
         <v xml:space="preserve">Interruptor pulsador de emergencia </v>
       </c>
-      <c r="J46" s="142"/>
-      <c r="K46" s="142"/>
-      <c r="L46" s="142"/>
+      <c r="J46" s="141"/>
+      <c r="K46" s="141"/>
+      <c r="L46" s="141"/>
       <c r="M46" s="139"/>
       <c r="N46" s="140"/>
       <c r="O46" s="140"/>
@@ -6837,13 +6837,13 @@
         <f>VLOOKUP(C48,Tbl_TiempoRespuestos[],3,0)</f>
         <v>1</v>
       </c>
-      <c r="I48" s="142" t="str">
+      <c r="I48" s="141" t="str">
         <f>C39</f>
         <v>Final de carrera superior</v>
       </c>
-      <c r="J48" s="142"/>
-      <c r="K48" s="142"/>
-      <c r="L48" s="142"/>
+      <c r="J48" s="141"/>
+      <c r="K48" s="141"/>
+      <c r="L48" s="141"/>
       <c r="M48" s="139"/>
       <c r="N48" s="140"/>
       <c r="O48" s="140"/>
@@ -6918,13 +6918,13 @@
         <f>VLOOKUP(C50,Tbl_TiempoRespuestos[],3,0)</f>
         <v>1</v>
       </c>
-      <c r="I50" s="142" t="str">
+      <c r="I50" s="141" t="str">
         <f>C40</f>
         <v>Final de carrera inferior</v>
       </c>
-      <c r="J50" s="142"/>
-      <c r="K50" s="142"/>
-      <c r="L50" s="142"/>
+      <c r="J50" s="141"/>
+      <c r="K50" s="141"/>
+      <c r="L50" s="141"/>
       <c r="M50" s="139"/>
       <c r="N50" s="140"/>
       <c r="O50" s="140"/>
@@ -6999,13 +6999,13 @@
         <f>VLOOKUP(C52,Tbl_TiempoRespuestos[],3,0)</f>
         <v>1</v>
       </c>
-      <c r="I52" s="142" t="str">
+      <c r="I52" s="141" t="str">
         <f>C41</f>
         <v>Final de carrera del sensor optico</v>
       </c>
-      <c r="J52" s="142"/>
-      <c r="K52" s="142"/>
-      <c r="L52" s="142"/>
+      <c r="J52" s="141"/>
+      <c r="K52" s="141"/>
+      <c r="L52" s="141"/>
       <c r="M52" s="139"/>
       <c r="N52" s="140"/>
       <c r="O52" s="140"/>
@@ -7041,20 +7041,20 @@
       </c>
     </row>
     <row r="54" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C54" s="136" t="s">
+      <c r="C54" s="153" t="s">
         <v>19</v>
       </c>
-      <c r="D54" s="136"/>
-      <c r="E54" s="136"/>
-      <c r="F54" s="136"/>
-      <c r="G54" s="136"/>
-      <c r="I54" s="141" t="str">
+      <c r="D54" s="153"/>
+      <c r="E54" s="153"/>
+      <c r="F54" s="153"/>
+      <c r="G54" s="153"/>
+      <c r="I54" s="172" t="str">
         <f>C42</f>
         <v>Kit de traba mecanica (traba, resorte, rotula, brazo regulador)</v>
       </c>
-      <c r="J54" s="141"/>
-      <c r="K54" s="141"/>
-      <c r="L54" s="141"/>
+      <c r="J54" s="172"/>
+      <c r="K54" s="172"/>
+      <c r="L54" s="172"/>
       <c r="M54" s="139"/>
       <c r="N54" s="140"/>
       <c r="O54" s="140"/>
@@ -7119,13 +7119,13 @@
       <c r="G56" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="I56" s="142" t="str">
+      <c r="I56" s="141" t="str">
         <f>C43</f>
         <v>Motor eléctrico (rebobinado)</v>
       </c>
-      <c r="J56" s="142"/>
-      <c r="K56" s="142"/>
-      <c r="L56" s="142"/>
+      <c r="J56" s="141"/>
+      <c r="K56" s="141"/>
+      <c r="L56" s="141"/>
       <c r="M56" s="139"/>
       <c r="N56" s="140"/>
       <c r="O56" s="140"/>
@@ -7190,13 +7190,13 @@
       <c r="G58" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="I58" s="142" t="str">
+      <c r="I58" s="141" t="str">
         <f>C44</f>
         <v>Piloto de señalización 220V</v>
       </c>
-      <c r="J58" s="142"/>
-      <c r="K58" s="142"/>
-      <c r="L58" s="142"/>
+      <c r="J58" s="141"/>
+      <c r="K58" s="141"/>
+      <c r="L58" s="141"/>
       <c r="M58" s="139"/>
       <c r="N58" s="140"/>
       <c r="O58" s="140"/>
@@ -7261,13 +7261,13 @@
       <c r="G60" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="I60" s="142" t="str">
+      <c r="I60" s="141" t="str">
         <f>C45</f>
         <v xml:space="preserve">Pulsador </v>
       </c>
-      <c r="J60" s="142"/>
-      <c r="K60" s="142"/>
-      <c r="L60" s="142"/>
+      <c r="J60" s="141"/>
+      <c r="K60" s="141"/>
+      <c r="L60" s="141"/>
       <c r="M60" s="139"/>
       <c r="N60" s="140"/>
       <c r="O60" s="140"/>
@@ -7333,13 +7333,13 @@
       <c r="G62" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="I62" s="142" t="str">
+      <c r="I62" s="141" t="str">
         <f>C46</f>
         <v>Relé encapsulado 220V 3A - 14 pines</v>
       </c>
-      <c r="J62" s="142"/>
-      <c r="K62" s="142"/>
-      <c r="L62" s="142"/>
+      <c r="J62" s="141"/>
+      <c r="K62" s="141"/>
+      <c r="L62" s="141"/>
       <c r="M62" s="139"/>
       <c r="N62" s="140"/>
       <c r="O62" s="140"/>
@@ -7406,13 +7406,13 @@
       <c r="G64" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="I64" s="142" t="str">
+      <c r="I64" s="141" t="str">
         <f>C47</f>
         <v>Selector rotativo - 3 posiciones</v>
       </c>
-      <c r="J64" s="142"/>
-      <c r="K64" s="142"/>
-      <c r="L64" s="142"/>
+      <c r="J64" s="141"/>
+      <c r="K64" s="141"/>
+      <c r="L64" s="141"/>
       <c r="M64" s="139"/>
       <c r="N64" s="140"/>
       <c r="O64" s="140"/>
@@ -7479,13 +7479,13 @@
       <c r="G66" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="I66" s="142" t="str">
+      <c r="I66" s="141" t="str">
         <f>C48</f>
         <v>Selector rotativo cerradura con llave</v>
       </c>
-      <c r="J66" s="142"/>
-      <c r="K66" s="142"/>
-      <c r="L66" s="142"/>
+      <c r="J66" s="141"/>
+      <c r="K66" s="141"/>
+      <c r="L66" s="141"/>
       <c r="M66" s="139"/>
       <c r="N66" s="140"/>
       <c r="O66" s="140"/>
@@ -7552,13 +7552,13 @@
       <c r="G68" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="I68" s="142" t="str">
+      <c r="I68" s="141" t="str">
         <f>C49</f>
         <v>Sensor óptico CHIIB</v>
       </c>
-      <c r="J68" s="142"/>
-      <c r="K68" s="142"/>
-      <c r="L68" s="142"/>
+      <c r="J68" s="141"/>
+      <c r="K68" s="141"/>
+      <c r="L68" s="141"/>
       <c r="M68" s="139"/>
       <c r="N68" s="140"/>
       <c r="O68" s="140"/>
@@ -7624,13 +7624,13 @@
       <c r="G70" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I70" s="142" t="str">
+      <c r="I70" s="141" t="str">
         <f>C50</f>
         <v>Solenoide de electroválvula</v>
       </c>
-      <c r="J70" s="142"/>
-      <c r="K70" s="142"/>
-      <c r="L70" s="142"/>
+      <c r="J70" s="141"/>
+      <c r="K70" s="141"/>
+      <c r="L70" s="141"/>
       <c r="M70" s="139"/>
       <c r="N70" s="140"/>
       <c r="O70" s="140"/>
@@ -7663,20 +7663,20 @@
       </c>
     </row>
     <row r="72" spans="3:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C72" s="136" t="s">
+      <c r="C72" s="153" t="s">
         <v>175</v>
       </c>
-      <c r="D72" s="136"/>
-      <c r="E72" s="136"/>
-      <c r="F72" s="136"/>
-      <c r="G72" s="136"/>
-      <c r="I72" s="142" t="str">
+      <c r="D72" s="153"/>
+      <c r="E72" s="153"/>
+      <c r="F72" s="153"/>
+      <c r="G72" s="153"/>
+      <c r="I72" s="141" t="str">
         <f>C51</f>
         <v>Solenoide de traba</v>
       </c>
-      <c r="J72" s="142"/>
-      <c r="K72" s="142"/>
-      <c r="L72" s="142"/>
+      <c r="J72" s="141"/>
+      <c r="K72" s="141"/>
+      <c r="L72" s="141"/>
       <c r="M72" s="139"/>
       <c r="N72" s="140"/>
       <c r="O72" s="140"/>
@@ -7731,13 +7731,13 @@
       <c r="E74" s="107"/>
       <c r="F74" s="107"/>
       <c r="G74" s="107"/>
-      <c r="I74" s="142" t="str">
+      <c r="I74" s="141" t="str">
         <f>C52</f>
         <v>Temporizador 220V</v>
       </c>
-      <c r="J74" s="142"/>
-      <c r="K74" s="142"/>
-      <c r="L74" s="142"/>
+      <c r="J74" s="141"/>
+      <c r="K74" s="141"/>
+      <c r="L74" s="141"/>
       <c r="M74" s="139"/>
       <c r="N74" s="140"/>
       <c r="O74" s="140"/>
@@ -7760,21 +7760,21 @@
       <c r="E76" s="107"/>
       <c r="F76" s="107"/>
       <c r="G76" s="107"/>
-      <c r="I76" s="143" t="s">
+      <c r="I76" s="144" t="s">
         <v>151</v>
       </c>
-      <c r="J76" s="144"/>
-      <c r="K76" s="144"/>
-      <c r="L76" s="145"/>
+      <c r="J76" s="145"/>
+      <c r="K76" s="145"/>
+      <c r="L76" s="146"/>
       <c r="M76" s="42">
         <f>SUM(M35:M74)</f>
         <v>2515</v>
       </c>
-      <c r="N76" s="146">
+      <c r="N76" s="147">
         <f>+SUM(N35:O74)</f>
         <v>754.5</v>
       </c>
-      <c r="O76" s="146"/>
+      <c r="O76" s="147"/>
       <c r="P76" s="29">
         <f>SUM(P35:P74)</f>
         <v>3269.5</v>
@@ -7797,12 +7797,12 @@
       <c r="E78" s="107"/>
       <c r="F78" s="107"/>
       <c r="G78" s="107"/>
-      <c r="I78" s="151" t="s">
+      <c r="I78" s="142" t="s">
         <v>152</v>
       </c>
-      <c r="J78" s="152"/>
-      <c r="K78" s="152"/>
-      <c r="L78" s="152"/>
+      <c r="J78" s="143"/>
+      <c r="K78" s="143"/>
+      <c r="L78" s="143"/>
     </row>
     <row r="79" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C79" s="99" t="s">
@@ -7812,12 +7812,12 @@
       <c r="E79" s="107"/>
       <c r="F79" s="107"/>
       <c r="G79" s="107"/>
-      <c r="I79" s="153" t="s">
+      <c r="I79" s="150" t="s">
         <v>142</v>
       </c>
-      <c r="J79" s="153"/>
-      <c r="K79" s="153"/>
-      <c r="L79" s="153"/>
+      <c r="J79" s="150"/>
+      <c r="K79" s="150"/>
+      <c r="L79" s="150"/>
       <c r="M79" s="86" t="s">
         <v>10</v>
       </c>
@@ -7873,13 +7873,13 @@
       <c r="E81" s="107"/>
       <c r="F81" s="107"/>
       <c r="G81" s="107"/>
-      <c r="I81" s="142" t="str">
+      <c r="I81" s="141" t="str">
         <f>C56</f>
         <v>Bolsa de basura 70 L (por unidad)</v>
       </c>
-      <c r="J81" s="142"/>
-      <c r="K81" s="142"/>
-      <c r="L81" s="142"/>
+      <c r="J81" s="141"/>
+      <c r="K81" s="141"/>
+      <c r="L81" s="141"/>
       <c r="M81" s="139"/>
       <c r="N81" s="140"/>
       <c r="O81" s="140"/>
@@ -7929,13 +7929,13 @@
       <c r="E83" s="107"/>
       <c r="F83" s="107"/>
       <c r="G83" s="107"/>
-      <c r="I83" s="142" t="str">
+      <c r="I83" s="141" t="str">
         <f>C57</f>
         <v xml:space="preserve">Cinta Aislante 1700 - 3M </v>
       </c>
-      <c r="J83" s="142"/>
-      <c r="K83" s="142"/>
-      <c r="L83" s="142"/>
+      <c r="J83" s="141"/>
+      <c r="K83" s="141"/>
+      <c r="L83" s="141"/>
       <c r="M83" s="139"/>
       <c r="N83" s="140"/>
       <c r="O83" s="140"/>
@@ -7983,13 +7983,13 @@
       <c r="E85" s="107"/>
       <c r="F85" s="107"/>
       <c r="G85" s="107"/>
-      <c r="I85" s="142" t="str">
+      <c r="I85" s="141" t="str">
         <f>C58</f>
         <v>Cinta reflectiva 3M (Amarillo) - 1 mts</v>
       </c>
-      <c r="J85" s="142"/>
-      <c r="K85" s="142"/>
-      <c r="L85" s="142"/>
+      <c r="J85" s="141"/>
+      <c r="K85" s="141"/>
+      <c r="L85" s="141"/>
       <c r="M85" s="139"/>
       <c r="N85" s="140"/>
       <c r="O85" s="140"/>
@@ -8037,13 +8037,13 @@
       <c r="E87" s="107"/>
       <c r="F87" s="107"/>
       <c r="G87" s="107"/>
-      <c r="I87" s="142" t="str">
+      <c r="I87" s="141" t="str">
         <f>C59</f>
         <v>Cintillo plástico 250 x 3.6 mm  (por unidad)</v>
       </c>
-      <c r="J87" s="142"/>
-      <c r="K87" s="142"/>
-      <c r="L87" s="142"/>
+      <c r="J87" s="141"/>
+      <c r="K87" s="141"/>
+      <c r="L87" s="141"/>
       <c r="M87" s="139"/>
       <c r="N87" s="140"/>
       <c r="O87" s="140"/>
@@ -8091,13 +8091,13 @@
       <c r="E89" s="107"/>
       <c r="F89" s="107"/>
       <c r="G89" s="107"/>
-      <c r="I89" s="142" t="str">
+      <c r="I89" s="141" t="str">
         <f>C60</f>
         <v>Cintillo plástico 370 x 4.8 mm  (por unidad)</v>
       </c>
-      <c r="J89" s="142"/>
-      <c r="K89" s="142"/>
-      <c r="L89" s="142"/>
+      <c r="J89" s="141"/>
+      <c r="K89" s="141"/>
+      <c r="L89" s="141"/>
       <c r="M89" s="139"/>
       <c r="N89" s="140"/>
       <c r="O89" s="140"/>
@@ -8145,13 +8145,13 @@
       <c r="E91" s="107"/>
       <c r="F91" s="107"/>
       <c r="G91" s="107"/>
-      <c r="I91" s="141" t="str">
+      <c r="I91" s="172" t="str">
         <f>C61</f>
         <v>Desengrasante industrial biodegradable - Hidrosol (1 gal)</v>
       </c>
-      <c r="J91" s="141"/>
-      <c r="K91" s="141"/>
-      <c r="L91" s="141"/>
+      <c r="J91" s="172"/>
+      <c r="K91" s="172"/>
+      <c r="L91" s="172"/>
       <c r="M91" s="139"/>
       <c r="N91" s="140"/>
       <c r="O91" s="140"/>
@@ -8199,13 +8199,13 @@
       <c r="E93" s="107"/>
       <c r="F93" s="107"/>
       <c r="G93" s="107"/>
-      <c r="I93" s="142" t="str">
+      <c r="I93" s="141" t="str">
         <f>C62</f>
         <v>Fusibles 5A - 100 und</v>
       </c>
-      <c r="J93" s="142"/>
-      <c r="K93" s="142"/>
-      <c r="L93" s="142"/>
+      <c r="J93" s="141"/>
+      <c r="K93" s="141"/>
+      <c r="L93" s="141"/>
       <c r="M93" s="139"/>
       <c r="N93" s="140"/>
       <c r="O93" s="140"/>
@@ -8239,13 +8239,13 @@
       </c>
     </row>
     <row r="95" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="I95" s="142" t="str">
+      <c r="I95" s="141" t="str">
         <f>C63</f>
         <v>Grasa en pasta (por kilo)</v>
       </c>
-      <c r="J95" s="142"/>
-      <c r="K95" s="142"/>
-      <c r="L95" s="142"/>
+      <c r="J95" s="141"/>
+      <c r="K95" s="141"/>
+      <c r="L95" s="141"/>
       <c r="M95" s="139"/>
       <c r="N95" s="140"/>
       <c r="O95" s="140"/>
@@ -8279,13 +8279,13 @@
       </c>
     </row>
     <row r="97" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I97" s="142" t="str">
+      <c r="I97" s="141" t="str">
         <f>C64</f>
         <v>Lija para metal #80</v>
       </c>
-      <c r="J97" s="142"/>
-      <c r="K97" s="142"/>
-      <c r="L97" s="142"/>
+      <c r="J97" s="141"/>
+      <c r="K97" s="141"/>
+      <c r="L97" s="141"/>
       <c r="M97" s="139"/>
       <c r="N97" s="140"/>
       <c r="O97" s="140"/>
@@ -8319,13 +8319,13 @@
       </c>
     </row>
     <row r="99" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I99" s="142" t="str">
+      <c r="I99" s="141" t="str">
         <f>C65</f>
         <v>Spray aerosol Alumnio - Rust Oleum</v>
       </c>
-      <c r="J99" s="142"/>
-      <c r="K99" s="142"/>
-      <c r="L99" s="142"/>
+      <c r="J99" s="141"/>
+      <c r="K99" s="141"/>
+      <c r="L99" s="141"/>
       <c r="M99" s="139"/>
       <c r="N99" s="140"/>
       <c r="O99" s="140"/>
@@ -8359,13 +8359,13 @@
       </c>
     </row>
     <row r="101" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I101" s="142" t="str">
+      <c r="I101" s="141" t="str">
         <f>C66</f>
         <v>Spray aerosol Negro - Rust Oleum</v>
       </c>
-      <c r="J101" s="142"/>
-      <c r="K101" s="142"/>
-      <c r="L101" s="142"/>
+      <c r="J101" s="141"/>
+      <c r="K101" s="141"/>
+      <c r="L101" s="141"/>
       <c r="M101" s="139"/>
       <c r="N101" s="140"/>
       <c r="O101" s="140"/>
@@ -8399,13 +8399,13 @@
       </c>
     </row>
     <row r="103" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I103" s="142" t="str">
+      <c r="I103" s="141" t="str">
         <f>C67</f>
         <v>Spray Aflojatodo 10 oz o 296 ml - VISTONY</v>
       </c>
-      <c r="J103" s="142"/>
-      <c r="K103" s="142"/>
-      <c r="L103" s="142"/>
+      <c r="J103" s="141"/>
+      <c r="K103" s="141"/>
+      <c r="L103" s="141"/>
       <c r="M103" s="139"/>
       <c r="N103" s="140"/>
       <c r="O103" s="140"/>
@@ -8439,13 +8439,13 @@
       </c>
     </row>
     <row r="105" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I105" s="142" t="str">
+      <c r="I105" s="141" t="str">
         <f>C68</f>
         <v>Spray Lubricante 10 oz o 296 ml - VISTONY</v>
       </c>
-      <c r="J105" s="142"/>
-      <c r="K105" s="142"/>
-      <c r="L105" s="142"/>
+      <c r="J105" s="141"/>
+      <c r="K105" s="141"/>
+      <c r="L105" s="141"/>
       <c r="M105" s="139"/>
       <c r="N105" s="140"/>
       <c r="O105" s="140"/>
@@ -8479,13 +8479,13 @@
       </c>
     </row>
     <row r="107" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I107" s="142" t="str">
+      <c r="I107" s="141" t="str">
         <f>C69</f>
         <v>Teflon</v>
       </c>
-      <c r="J107" s="142"/>
-      <c r="K107" s="142"/>
-      <c r="L107" s="142"/>
+      <c r="J107" s="141"/>
+      <c r="K107" s="141"/>
+      <c r="L107" s="141"/>
       <c r="M107" s="139"/>
       <c r="N107" s="140"/>
       <c r="O107" s="140"/>
@@ -8519,54 +8519,54 @@
       </c>
     </row>
     <row r="109" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I109" s="142" t="str">
+      <c r="I109" s="141" t="str">
         <f>C70</f>
         <v>Trapos Industriales (por kilo)</v>
       </c>
-      <c r="J109" s="142"/>
-      <c r="K109" s="142"/>
-      <c r="L109" s="142"/>
+      <c r="J109" s="141"/>
+      <c r="K109" s="141"/>
+      <c r="L109" s="141"/>
       <c r="M109" s="139"/>
       <c r="N109" s="140"/>
       <c r="O109" s="140"/>
       <c r="P109" s="140"/>
     </row>
     <row r="111" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I111" s="143" t="s">
+      <c r="I111" s="144" t="s">
         <v>159</v>
       </c>
-      <c r="J111" s="144"/>
-      <c r="K111" s="144"/>
-      <c r="L111" s="145"/>
+      <c r="J111" s="145"/>
+      <c r="K111" s="145"/>
+      <c r="L111" s="146"/>
       <c r="M111" s="64">
         <f>SUM(M80:M109)</f>
         <v>1194.5</v>
       </c>
-      <c r="N111" s="146">
+      <c r="N111" s="147">
         <f>+SUM(N80:O109)</f>
         <v>358.35</v>
       </c>
-      <c r="O111" s="146"/>
+      <c r="O111" s="147"/>
       <c r="P111" s="29">
         <f>SUM(P80:P109)</f>
         <v>1552.85</v>
       </c>
     </row>
     <row r="113" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I113" s="151" t="s">
+      <c r="I113" s="142" t="s">
         <v>153</v>
       </c>
-      <c r="J113" s="152"/>
-      <c r="K113" s="152"/>
-      <c r="L113" s="152"/>
+      <c r="J113" s="143"/>
+      <c r="K113" s="143"/>
+      <c r="L113" s="143"/>
     </row>
     <row r="114" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I114" s="153" t="s">
+      <c r="I114" s="150" t="s">
         <v>142</v>
       </c>
-      <c r="J114" s="153"/>
-      <c r="K114" s="153"/>
-      <c r="L114" s="153"/>
+      <c r="J114" s="150"/>
+      <c r="K114" s="150"/>
+      <c r="L114" s="150"/>
       <c r="M114" s="86" t="s">
         <v>10</v>
       </c>
@@ -8607,12 +8607,12 @@
       </c>
     </row>
     <row r="116" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I116" s="142" t="s">
+      <c r="I116" s="141" t="s">
         <v>13</v>
       </c>
-      <c r="J116" s="142"/>
-      <c r="K116" s="142"/>
-      <c r="L116" s="142"/>
+      <c r="J116" s="141"/>
+      <c r="K116" s="141"/>
+      <c r="L116" s="141"/>
       <c r="M116" s="139"/>
       <c r="N116" s="140"/>
       <c r="O116" s="140"/>
@@ -8645,12 +8645,12 @@
       </c>
     </row>
     <row r="118" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I118" s="142" t="s">
+      <c r="I118" s="141" t="s">
         <v>38</v>
       </c>
-      <c r="J118" s="142"/>
-      <c r="K118" s="142"/>
-      <c r="L118" s="142"/>
+      <c r="J118" s="141"/>
+      <c r="K118" s="141"/>
+      <c r="L118" s="141"/>
       <c r="M118" s="139"/>
       <c r="N118" s="140"/>
       <c r="O118" s="140"/>
@@ -8683,12 +8683,12 @@
       </c>
     </row>
     <row r="120" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I120" s="142" t="s">
+      <c r="I120" s="141" t="s">
         <v>98</v>
       </c>
-      <c r="J120" s="142"/>
-      <c r="K120" s="142"/>
-      <c r="L120" s="142"/>
+      <c r="J120" s="141"/>
+      <c r="K120" s="141"/>
+      <c r="L120" s="141"/>
       <c r="M120" s="139"/>
       <c r="N120" s="140"/>
       <c r="O120" s="140"/>
@@ -8721,12 +8721,12 @@
       </c>
     </row>
     <row r="122" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I122" s="142" t="s">
+      <c r="I122" s="141" t="s">
         <v>101</v>
       </c>
-      <c r="J122" s="142"/>
-      <c r="K122" s="142"/>
-      <c r="L122" s="142"/>
+      <c r="J122" s="141"/>
+      <c r="K122" s="141"/>
+      <c r="L122" s="141"/>
       <c r="M122" s="139"/>
       <c r="N122" s="140"/>
       <c r="O122" s="140"/>
@@ -8759,12 +8759,12 @@
       </c>
     </row>
     <row r="124" spans="9:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I124" s="142" t="s">
+      <c r="I124" s="141" t="s">
         <v>100</v>
       </c>
-      <c r="J124" s="142"/>
-      <c r="K124" s="142"/>
-      <c r="L124" s="142"/>
+      <c r="J124" s="141"/>
+      <c r="K124" s="141"/>
+      <c r="L124" s="141"/>
       <c r="M124" s="139"/>
       <c r="N124" s="140"/>
       <c r="O124" s="140"/>
@@ -8772,21 +8772,21 @@
     </row>
     <row r="125" spans="9:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="126" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I126" s="143" t="s">
+      <c r="I126" s="144" t="s">
         <v>158</v>
       </c>
-      <c r="J126" s="144"/>
-      <c r="K126" s="144"/>
-      <c r="L126" s="145"/>
+      <c r="J126" s="145"/>
+      <c r="K126" s="145"/>
+      <c r="L126" s="146"/>
       <c r="M126" s="64">
         <f>SUM(M115:M124)</f>
         <v>684</v>
       </c>
-      <c r="N126" s="146">
+      <c r="N126" s="147">
         <f>+SUM(N115:O124)</f>
         <v>205.2</v>
       </c>
-      <c r="O126" s="146"/>
+      <c r="O126" s="147"/>
       <c r="P126" s="29">
         <f>SUM(P115:P124)</f>
         <v>889.2</v>
@@ -8804,21 +8804,21 @@
     </row>
     <row r="128" spans="9:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="129" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I129" s="147" t="s">
+      <c r="I129" s="168" t="s">
         <v>154</v>
       </c>
-      <c r="J129" s="148"/>
-      <c r="K129" s="148"/>
-      <c r="L129" s="149"/>
+      <c r="J129" s="169"/>
+      <c r="K129" s="169"/>
+      <c r="L129" s="170"/>
       <c r="M129" s="91">
         <f>SUM(M18,M31,M76,M111,M126)</f>
         <v>10065.139435763889</v>
       </c>
-      <c r="N129" s="150">
+      <c r="N129" s="171">
         <f>SUM(N18,N31,N76,N111,N126)</f>
         <v>3465.0697178819437</v>
       </c>
-      <c r="O129" s="149"/>
+      <c r="O129" s="170"/>
       <c r="P129" s="91">
         <f>SUM(P18,P31,P76,P111,P126)</f>
         <v>13530.209153645834</v>
@@ -8831,17 +8831,17 @@
       <c r="P130" s="22"/>
     </row>
     <row r="131" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I131" s="154" t="s">
+      <c r="I131" s="161" t="s">
         <v>155</v>
       </c>
-      <c r="J131" s="155"/>
-      <c r="K131" s="156"/>
+      <c r="J131" s="162"/>
+      <c r="K131" s="163"/>
       <c r="L131" s="93">
         <v>0.05</v>
       </c>
-      <c r="M131" s="157"/>
-      <c r="N131" s="158"/>
-      <c r="O131" s="159"/>
+      <c r="M131" s="164"/>
+      <c r="N131" s="165"/>
+      <c r="O131" s="166"/>
       <c r="P131" s="94">
         <f>P129*L131</f>
         <v>676.51045768229176</v>
@@ -8854,15 +8854,15 @@
       <c r="P132" s="22"/>
     </row>
     <row r="133" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I133" s="160" t="s">
+      <c r="I133" s="167" t="s">
         <v>156</v>
       </c>
-      <c r="J133" s="160"/>
-      <c r="K133" s="160"/>
-      <c r="L133" s="160"/>
-      <c r="M133" s="160"/>
-      <c r="N133" s="160"/>
-      <c r="O133" s="160"/>
+      <c r="J133" s="167"/>
+      <c r="K133" s="167"/>
+      <c r="L133" s="167"/>
+      <c r="M133" s="167"/>
+      <c r="N133" s="167"/>
+      <c r="O133" s="167"/>
       <c r="P133" s="95">
         <f>SUM(P129:P131)</f>
         <v>14206.719611328126</v>
@@ -8873,16 +8873,242 @@
     <sortCondition ref="C57"/>
   </sortState>
   <mergeCells count="270">
-    <mergeCell ref="I104:J104"/>
-    <mergeCell ref="M104:M105"/>
-    <mergeCell ref="N104:O105"/>
-    <mergeCell ref="P104:P105"/>
-    <mergeCell ref="I105:L105"/>
-    <mergeCell ref="I106:J106"/>
-    <mergeCell ref="M106:M107"/>
-    <mergeCell ref="N106:O107"/>
-    <mergeCell ref="P106:P107"/>
-    <mergeCell ref="I107:L107"/>
+    <mergeCell ref="C72:G72"/>
+    <mergeCell ref="I53:J53"/>
+    <mergeCell ref="M53:M54"/>
+    <mergeCell ref="N53:O54"/>
+    <mergeCell ref="P53:P54"/>
+    <mergeCell ref="I54:L54"/>
+    <mergeCell ref="I90:J90"/>
+    <mergeCell ref="M90:M91"/>
+    <mergeCell ref="N90:O91"/>
+    <mergeCell ref="P90:P91"/>
+    <mergeCell ref="I91:L91"/>
+    <mergeCell ref="I86:J86"/>
+    <mergeCell ref="M86:M87"/>
+    <mergeCell ref="N86:O87"/>
+    <mergeCell ref="P86:P87"/>
+    <mergeCell ref="I87:L87"/>
+    <mergeCell ref="I88:J88"/>
+    <mergeCell ref="M88:M89"/>
+    <mergeCell ref="N88:O89"/>
+    <mergeCell ref="P88:P89"/>
+    <mergeCell ref="I89:L89"/>
+    <mergeCell ref="I82:J82"/>
+    <mergeCell ref="M82:M83"/>
+    <mergeCell ref="N82:O83"/>
+    <mergeCell ref="M92:M93"/>
+    <mergeCell ref="N92:O93"/>
+    <mergeCell ref="P92:P93"/>
+    <mergeCell ref="I93:L93"/>
+    <mergeCell ref="M41:M42"/>
+    <mergeCell ref="N41:O42"/>
+    <mergeCell ref="P41:P42"/>
+    <mergeCell ref="I42:L42"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="M59:M60"/>
+    <mergeCell ref="N59:O60"/>
+    <mergeCell ref="P59:P60"/>
+    <mergeCell ref="I60:L60"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="M43:M44"/>
+    <mergeCell ref="N43:O44"/>
+    <mergeCell ref="P43:P44"/>
+    <mergeCell ref="I44:L44"/>
+    <mergeCell ref="I67:J67"/>
+    <mergeCell ref="M67:M68"/>
+    <mergeCell ref="N67:O68"/>
+    <mergeCell ref="P67:P68"/>
+    <mergeCell ref="I68:L68"/>
+    <mergeCell ref="M45:M46"/>
+    <mergeCell ref="N45:O46"/>
+    <mergeCell ref="P45:P46"/>
+    <mergeCell ref="I46:L46"/>
+    <mergeCell ref="I126:L126"/>
+    <mergeCell ref="N126:O126"/>
+    <mergeCell ref="I129:L129"/>
+    <mergeCell ref="N129:O129"/>
+    <mergeCell ref="P115:P116"/>
+    <mergeCell ref="P121:P122"/>
+    <mergeCell ref="P123:P124"/>
+    <mergeCell ref="P117:P118"/>
+    <mergeCell ref="P119:P120"/>
+    <mergeCell ref="I102:J102"/>
+    <mergeCell ref="M102:M103"/>
+    <mergeCell ref="N102:O103"/>
+    <mergeCell ref="P102:P103"/>
+    <mergeCell ref="I103:L103"/>
+    <mergeCell ref="I111:L111"/>
+    <mergeCell ref="N111:O111"/>
+    <mergeCell ref="I113:L113"/>
+    <mergeCell ref="I114:L114"/>
+    <mergeCell ref="I98:J98"/>
+    <mergeCell ref="I92:J92"/>
+    <mergeCell ref="M98:M99"/>
+    <mergeCell ref="I131:K131"/>
+    <mergeCell ref="M131:O131"/>
+    <mergeCell ref="I133:O133"/>
+    <mergeCell ref="I121:J121"/>
+    <mergeCell ref="M121:M122"/>
+    <mergeCell ref="N121:O122"/>
+    <mergeCell ref="I115:J115"/>
+    <mergeCell ref="M115:M116"/>
+    <mergeCell ref="N115:O116"/>
+    <mergeCell ref="I116:L116"/>
+    <mergeCell ref="I122:L122"/>
+    <mergeCell ref="I123:J123"/>
+    <mergeCell ref="M123:M124"/>
+    <mergeCell ref="N123:O124"/>
+    <mergeCell ref="I124:L124"/>
+    <mergeCell ref="I117:J117"/>
+    <mergeCell ref="M117:M118"/>
+    <mergeCell ref="N117:O118"/>
+    <mergeCell ref="I118:L118"/>
+    <mergeCell ref="I119:J119"/>
+    <mergeCell ref="M119:M120"/>
+    <mergeCell ref="N119:O120"/>
+    <mergeCell ref="I120:L120"/>
+    <mergeCell ref="N98:O99"/>
+    <mergeCell ref="P98:P99"/>
+    <mergeCell ref="I99:L99"/>
+    <mergeCell ref="I100:J100"/>
+    <mergeCell ref="M100:M101"/>
+    <mergeCell ref="N100:O101"/>
+    <mergeCell ref="P100:P101"/>
+    <mergeCell ref="I101:L101"/>
+    <mergeCell ref="I94:J94"/>
+    <mergeCell ref="M94:M95"/>
+    <mergeCell ref="N94:O95"/>
+    <mergeCell ref="P94:P95"/>
+    <mergeCell ref="I95:L95"/>
+    <mergeCell ref="I96:J96"/>
+    <mergeCell ref="M96:M97"/>
+    <mergeCell ref="N96:O97"/>
+    <mergeCell ref="P96:P97"/>
+    <mergeCell ref="I97:L97"/>
+    <mergeCell ref="P82:P83"/>
+    <mergeCell ref="I83:L83"/>
+    <mergeCell ref="I84:J84"/>
+    <mergeCell ref="M84:M85"/>
+    <mergeCell ref="N84:O85"/>
+    <mergeCell ref="P84:P85"/>
+    <mergeCell ref="I85:L85"/>
+    <mergeCell ref="I73:J73"/>
+    <mergeCell ref="M73:M74"/>
+    <mergeCell ref="N73:O74"/>
+    <mergeCell ref="P73:P74"/>
+    <mergeCell ref="I74:L74"/>
+    <mergeCell ref="I78:L78"/>
+    <mergeCell ref="I79:L79"/>
+    <mergeCell ref="I80:J80"/>
+    <mergeCell ref="M80:M81"/>
+    <mergeCell ref="N80:O81"/>
+    <mergeCell ref="P80:P81"/>
+    <mergeCell ref="I81:L81"/>
+    <mergeCell ref="I76:L76"/>
+    <mergeCell ref="N76:O76"/>
+    <mergeCell ref="I69:J69"/>
+    <mergeCell ref="M69:M70"/>
+    <mergeCell ref="N69:O70"/>
+    <mergeCell ref="P69:P70"/>
+    <mergeCell ref="I70:L70"/>
+    <mergeCell ref="I71:J71"/>
+    <mergeCell ref="M71:M72"/>
+    <mergeCell ref="N71:O72"/>
+    <mergeCell ref="P71:P72"/>
+    <mergeCell ref="I72:L72"/>
+    <mergeCell ref="I63:J63"/>
+    <mergeCell ref="M63:M64"/>
+    <mergeCell ref="N63:O64"/>
+    <mergeCell ref="P63:P64"/>
+    <mergeCell ref="I64:L64"/>
+    <mergeCell ref="I65:J65"/>
+    <mergeCell ref="M65:M66"/>
+    <mergeCell ref="N65:O66"/>
+    <mergeCell ref="P65:P66"/>
+    <mergeCell ref="I66:L66"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C54:G54"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="I10:L10"/>
+    <mergeCell ref="I12:L12"/>
+    <mergeCell ref="I18:L18"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="I34:L34"/>
+    <mergeCell ref="I51:J51"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="N13:O14"/>
+    <mergeCell ref="P13:P14"/>
+    <mergeCell ref="I14:L14"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="N15:O16"/>
+    <mergeCell ref="P15:P16"/>
+    <mergeCell ref="I16:L16"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:O10"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="N11:O12"/>
+    <mergeCell ref="P11:P12"/>
+    <mergeCell ref="M24:M25"/>
+    <mergeCell ref="N24:O25"/>
+    <mergeCell ref="P24:P25"/>
+    <mergeCell ref="I25:L25"/>
+    <mergeCell ref="M26:M27"/>
+    <mergeCell ref="N26:O27"/>
+    <mergeCell ref="P26:P27"/>
+    <mergeCell ref="I27:L27"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="I21:L21"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="N22:O23"/>
+    <mergeCell ref="P22:P23"/>
+    <mergeCell ref="I23:L23"/>
+    <mergeCell ref="M35:M36"/>
+    <mergeCell ref="N35:O36"/>
+    <mergeCell ref="P35:P36"/>
+    <mergeCell ref="I36:L36"/>
+    <mergeCell ref="I33:L33"/>
+    <mergeCell ref="I31:L31"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="M28:M29"/>
+    <mergeCell ref="N28:O29"/>
+    <mergeCell ref="P28:P29"/>
+    <mergeCell ref="I29:L29"/>
+    <mergeCell ref="N37:O38"/>
+    <mergeCell ref="M37:M38"/>
+    <mergeCell ref="P37:P38"/>
+    <mergeCell ref="I38:L38"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="M39:M40"/>
+    <mergeCell ref="N39:O40"/>
+    <mergeCell ref="P39:P40"/>
+    <mergeCell ref="I40:L40"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="M49:M50"/>
+    <mergeCell ref="N49:O50"/>
+    <mergeCell ref="P49:P50"/>
+    <mergeCell ref="I50:L50"/>
+    <mergeCell ref="I49:J49"/>
+    <mergeCell ref="M47:M48"/>
+    <mergeCell ref="N47:O48"/>
+    <mergeCell ref="P47:P48"/>
+    <mergeCell ref="I48:L48"/>
+    <mergeCell ref="I47:J47"/>
     <mergeCell ref="M51:M52"/>
     <mergeCell ref="N51:O52"/>
     <mergeCell ref="P51:P52"/>
@@ -8907,242 +9133,16 @@
     <mergeCell ref="N61:O62"/>
     <mergeCell ref="P61:P62"/>
     <mergeCell ref="I62:L62"/>
-    <mergeCell ref="M49:M50"/>
-    <mergeCell ref="N49:O50"/>
-    <mergeCell ref="P49:P50"/>
-    <mergeCell ref="I50:L50"/>
-    <mergeCell ref="I49:J49"/>
-    <mergeCell ref="M47:M48"/>
-    <mergeCell ref="N47:O48"/>
-    <mergeCell ref="P47:P48"/>
-    <mergeCell ref="I48:L48"/>
-    <mergeCell ref="I47:J47"/>
-    <mergeCell ref="N37:O38"/>
-    <mergeCell ref="M37:M38"/>
-    <mergeCell ref="P37:P38"/>
-    <mergeCell ref="I38:L38"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="M39:M40"/>
-    <mergeCell ref="N39:O40"/>
-    <mergeCell ref="P39:P40"/>
-    <mergeCell ref="I40:L40"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="M35:M36"/>
-    <mergeCell ref="N35:O36"/>
-    <mergeCell ref="P35:P36"/>
-    <mergeCell ref="I36:L36"/>
-    <mergeCell ref="I33:L33"/>
-    <mergeCell ref="I31:L31"/>
-    <mergeCell ref="N31:O31"/>
-    <mergeCell ref="M28:M29"/>
-    <mergeCell ref="N28:O29"/>
-    <mergeCell ref="P28:P29"/>
-    <mergeCell ref="I29:L29"/>
-    <mergeCell ref="M24:M25"/>
-    <mergeCell ref="N24:O25"/>
-    <mergeCell ref="P24:P25"/>
-    <mergeCell ref="I25:L25"/>
-    <mergeCell ref="M26:M27"/>
-    <mergeCell ref="N26:O27"/>
-    <mergeCell ref="P26:P27"/>
-    <mergeCell ref="I27:L27"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="I21:L21"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="N22:O23"/>
-    <mergeCell ref="P22:P23"/>
-    <mergeCell ref="I23:L23"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="N13:O14"/>
-    <mergeCell ref="P13:P14"/>
-    <mergeCell ref="I14:L14"/>
-    <mergeCell ref="M15:M16"/>
-    <mergeCell ref="N15:O16"/>
-    <mergeCell ref="P15:P16"/>
-    <mergeCell ref="I16:L16"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:O10"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="N11:O12"/>
-    <mergeCell ref="P11:P12"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C54:G54"/>
-    <mergeCell ref="I8:L8"/>
-    <mergeCell ref="I10:L10"/>
-    <mergeCell ref="I12:L12"/>
-    <mergeCell ref="I18:L18"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="I34:L34"/>
-    <mergeCell ref="I51:J51"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="I63:J63"/>
-    <mergeCell ref="M63:M64"/>
-    <mergeCell ref="N63:O64"/>
-    <mergeCell ref="P63:P64"/>
-    <mergeCell ref="I64:L64"/>
-    <mergeCell ref="I65:J65"/>
-    <mergeCell ref="M65:M66"/>
-    <mergeCell ref="N65:O66"/>
-    <mergeCell ref="P65:P66"/>
-    <mergeCell ref="I66:L66"/>
-    <mergeCell ref="I69:J69"/>
-    <mergeCell ref="M69:M70"/>
-    <mergeCell ref="N69:O70"/>
-    <mergeCell ref="P69:P70"/>
-    <mergeCell ref="I70:L70"/>
-    <mergeCell ref="I71:J71"/>
-    <mergeCell ref="M71:M72"/>
-    <mergeCell ref="N71:O72"/>
-    <mergeCell ref="P71:P72"/>
-    <mergeCell ref="I72:L72"/>
-    <mergeCell ref="P82:P83"/>
-    <mergeCell ref="I83:L83"/>
-    <mergeCell ref="I84:J84"/>
-    <mergeCell ref="M84:M85"/>
-    <mergeCell ref="N84:O85"/>
-    <mergeCell ref="P84:P85"/>
-    <mergeCell ref="I85:L85"/>
-    <mergeCell ref="I73:J73"/>
-    <mergeCell ref="M73:M74"/>
-    <mergeCell ref="N73:O74"/>
-    <mergeCell ref="P73:P74"/>
-    <mergeCell ref="I74:L74"/>
-    <mergeCell ref="I78:L78"/>
-    <mergeCell ref="I79:L79"/>
-    <mergeCell ref="I80:J80"/>
-    <mergeCell ref="M80:M81"/>
-    <mergeCell ref="N80:O81"/>
-    <mergeCell ref="P80:P81"/>
-    <mergeCell ref="I81:L81"/>
-    <mergeCell ref="I76:L76"/>
-    <mergeCell ref="N76:O76"/>
-    <mergeCell ref="N98:O99"/>
-    <mergeCell ref="P98:P99"/>
-    <mergeCell ref="I99:L99"/>
-    <mergeCell ref="I100:J100"/>
-    <mergeCell ref="M100:M101"/>
-    <mergeCell ref="N100:O101"/>
-    <mergeCell ref="P100:P101"/>
-    <mergeCell ref="I101:L101"/>
-    <mergeCell ref="I94:J94"/>
-    <mergeCell ref="M94:M95"/>
-    <mergeCell ref="N94:O95"/>
-    <mergeCell ref="P94:P95"/>
-    <mergeCell ref="I95:L95"/>
-    <mergeCell ref="I96:J96"/>
-    <mergeCell ref="M96:M97"/>
-    <mergeCell ref="N96:O97"/>
-    <mergeCell ref="P96:P97"/>
-    <mergeCell ref="I97:L97"/>
-    <mergeCell ref="I131:K131"/>
-    <mergeCell ref="M131:O131"/>
-    <mergeCell ref="I133:O133"/>
-    <mergeCell ref="I121:J121"/>
-    <mergeCell ref="M121:M122"/>
-    <mergeCell ref="N121:O122"/>
-    <mergeCell ref="I115:J115"/>
-    <mergeCell ref="M115:M116"/>
-    <mergeCell ref="N115:O116"/>
-    <mergeCell ref="I116:L116"/>
-    <mergeCell ref="I122:L122"/>
-    <mergeCell ref="I123:J123"/>
-    <mergeCell ref="M123:M124"/>
-    <mergeCell ref="N123:O124"/>
-    <mergeCell ref="I124:L124"/>
-    <mergeCell ref="I117:J117"/>
-    <mergeCell ref="M117:M118"/>
-    <mergeCell ref="N117:O118"/>
-    <mergeCell ref="I118:L118"/>
-    <mergeCell ref="I119:J119"/>
-    <mergeCell ref="M119:M120"/>
-    <mergeCell ref="N119:O120"/>
-    <mergeCell ref="I120:L120"/>
-    <mergeCell ref="N45:O46"/>
-    <mergeCell ref="P45:P46"/>
-    <mergeCell ref="I46:L46"/>
-    <mergeCell ref="I126:L126"/>
-    <mergeCell ref="N126:O126"/>
-    <mergeCell ref="I129:L129"/>
-    <mergeCell ref="N129:O129"/>
-    <mergeCell ref="P115:P116"/>
-    <mergeCell ref="P121:P122"/>
-    <mergeCell ref="P123:P124"/>
-    <mergeCell ref="P117:P118"/>
-    <mergeCell ref="P119:P120"/>
-    <mergeCell ref="I102:J102"/>
-    <mergeCell ref="M102:M103"/>
-    <mergeCell ref="N102:O103"/>
-    <mergeCell ref="P102:P103"/>
-    <mergeCell ref="I103:L103"/>
-    <mergeCell ref="I111:L111"/>
-    <mergeCell ref="N111:O111"/>
-    <mergeCell ref="I113:L113"/>
-    <mergeCell ref="I114:L114"/>
-    <mergeCell ref="I98:J98"/>
-    <mergeCell ref="I92:J92"/>
-    <mergeCell ref="M98:M99"/>
-    <mergeCell ref="M92:M93"/>
-    <mergeCell ref="N92:O93"/>
-    <mergeCell ref="P92:P93"/>
-    <mergeCell ref="I93:L93"/>
-    <mergeCell ref="M41:M42"/>
-    <mergeCell ref="N41:O42"/>
-    <mergeCell ref="P41:P42"/>
-    <mergeCell ref="I42:L42"/>
-    <mergeCell ref="I59:J59"/>
-    <mergeCell ref="M59:M60"/>
-    <mergeCell ref="N59:O60"/>
-    <mergeCell ref="P59:P60"/>
-    <mergeCell ref="I60:L60"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="M43:M44"/>
-    <mergeCell ref="N43:O44"/>
-    <mergeCell ref="P43:P44"/>
-    <mergeCell ref="I44:L44"/>
-    <mergeCell ref="I67:J67"/>
-    <mergeCell ref="M67:M68"/>
-    <mergeCell ref="N67:O68"/>
-    <mergeCell ref="P67:P68"/>
-    <mergeCell ref="I68:L68"/>
-    <mergeCell ref="M45:M46"/>
-    <mergeCell ref="C72:G72"/>
-    <mergeCell ref="I53:J53"/>
-    <mergeCell ref="M53:M54"/>
-    <mergeCell ref="N53:O54"/>
-    <mergeCell ref="P53:P54"/>
-    <mergeCell ref="I54:L54"/>
-    <mergeCell ref="I90:J90"/>
-    <mergeCell ref="M90:M91"/>
-    <mergeCell ref="N90:O91"/>
-    <mergeCell ref="P90:P91"/>
-    <mergeCell ref="I91:L91"/>
-    <mergeCell ref="I86:J86"/>
-    <mergeCell ref="M86:M87"/>
-    <mergeCell ref="N86:O87"/>
-    <mergeCell ref="P86:P87"/>
-    <mergeCell ref="I87:L87"/>
-    <mergeCell ref="I88:J88"/>
-    <mergeCell ref="M88:M89"/>
-    <mergeCell ref="N88:O89"/>
-    <mergeCell ref="P88:P89"/>
-    <mergeCell ref="I89:L89"/>
-    <mergeCell ref="I82:J82"/>
-    <mergeCell ref="M82:M83"/>
-    <mergeCell ref="N82:O83"/>
+    <mergeCell ref="I104:J104"/>
+    <mergeCell ref="M104:M105"/>
+    <mergeCell ref="N104:O105"/>
+    <mergeCell ref="P104:P105"/>
+    <mergeCell ref="I105:L105"/>
+    <mergeCell ref="I106:J106"/>
+    <mergeCell ref="M106:M107"/>
+    <mergeCell ref="N106:O107"/>
+    <mergeCell ref="P106:P107"/>
+    <mergeCell ref="I107:L107"/>
   </mergeCells>
   <conditionalFormatting sqref="D33:D52">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
@@ -9152,7 +9152,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="5">
+  <dataValidations disablePrompts="1" count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C26:C29 C33:C52 C83">
       <formula1>TiempoRepuesto</formula1>
     </dataValidation>
@@ -9177,7 +9177,7 @@
   </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>COSTOS!$B$4:$B$35</xm:f>

</xml_diff>